<commit_message>
plik naglowkowy + doxygen
</commit_message>
<xml_diff>
--- a/protocol/protocol_b.xlsx
+++ b/protocol/protocol_b.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Death Freak\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="21072" windowHeight="9528"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="21075" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
     <sheet name="UDP-TCP" sheetId="2" r:id="rId2"/>
     <sheet name="Configuration" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="153">
   <si>
     <t>UDP</t>
   </si>
@@ -143,18 +138,9 @@
     <t>E* - enum</t>
   </si>
   <si>
-    <t>UProtocolType</t>
-  </si>
-  <si>
     <t>Uwagi:</t>
   </si>
   <si>
-    <t>EProtocolType</t>
-  </si>
-  <si>
-    <t>EProtocolType definiuje opcje w UProtocolType</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
@@ -200,9 +186,6 @@
     <t xml:space="preserve"> &lt;-&gt; w obie strony</t>
   </si>
   <si>
-    <t>EProtocolType &lt;-&gt;</t>
-  </si>
-  <si>
     <t>MONITOR_DATA -&gt;</t>
   </si>
   <si>
@@ -215,9 +198,6 @@
     <t>SConfigurationResponse -&gt;</t>
   </si>
   <si>
-    <t>UProtocolType &lt;-&gt;</t>
-  </si>
-  <si>
     <t>SSensorData -&gt;</t>
   </si>
   <si>
@@ -483,6 +463,18 @@
   </si>
   <si>
     <t>Krzysiek: sądzę że lepiej użyć TCP. Czytałem że lepiej zabezpiecza przekaz danych i uodparnia od ewentualnych problemów z docieraniem ramek</t>
+  </si>
+  <si>
+    <t>EMessageType</t>
+  </si>
+  <si>
+    <t>EMessageType &lt;-&gt;</t>
+  </si>
+  <si>
+    <t>Umessage</t>
+  </si>
+  <si>
+    <t>UMessage &lt;-&gt;</t>
   </si>
 </sst>
 </file>
@@ -1198,6 +1190,156 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1210,15 +1352,6 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1232,147 +1365,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1435,7 +1427,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1470,7 +1462,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1681,112 +1673,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>144</v>
-      </c>
       <c r="C4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="111"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="112"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="74"/>
+    </row>
+    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="32"/>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -1799,22 +1791,22 @@
       <c r="J15" s="31"/>
       <c r="K15" s="44"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="113" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
+    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
       <c r="H16" s="60"/>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
       <c r="K16" s="44"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>2</v>
       </c>
@@ -1828,21 +1820,21 @@
         <v>5</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="44"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>6</v>
@@ -1852,7 +1844,7 @@
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>8</v>
@@ -1864,13 +1856,13 @@
       <c r="J18" s="31"/>
       <c r="K18" s="44"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
-      <c r="E19" s="115" t="s">
-        <v>130</v>
+      <c r="E19" s="77" t="s">
+        <v>125</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>10</v>
@@ -1880,12 +1872,12 @@
       <c r="J19" s="31"/>
       <c r="K19" s="44"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="115"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="24" t="s">
         <v>11</v>
       </c>
@@ -1894,49 +1886,49 @@
       <c r="J20" s="31"/>
       <c r="K20" s="44"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
-      <c r="E21" s="115"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G21" s="24"/>
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
       <c r="K21" s="44"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
-      <c r="E22" s="115"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G22" s="24"/>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
       <c r="K22" s="44"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
       <c r="E23" s="31"/>
       <c r="F23" s="24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G23" s="24"/>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
       <c r="K23" s="44"/>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="23"/>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -1950,21 +1942,21 @@
       <c r="K24" s="44"/>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="78"/>
+      <c r="A25" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="91"/>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
       <c r="K25" s="44"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="31"/>
@@ -1977,14 +1969,14 @@
       <c r="J26" s="31"/>
       <c r="K26" s="44"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="84" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="85"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="97"/>
       <c r="C27" s="15"/>
       <c r="D27" s="28" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E27" s="31"/>
       <c r="F27" s="24"/>
@@ -1994,12 +1986,12 @@
       <c r="J27" s="31"/>
       <c r="K27" s="44"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -2011,9 +2003,9 @@
       <c r="J28" s="31"/>
       <c r="K28" s="44"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>18</v>
@@ -2028,7 +2020,7 @@
       <c r="J29" s="31"/>
       <c r="K29" s="44"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2041,12 +2033,12 @@
       <c r="J30" s="31"/>
       <c r="K30" s="44"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="90" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="91"/>
-      <c r="C31" s="91"/>
+    <row r="31" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A31" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="28"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -2056,12 +2048,12 @@
       <c r="J31" s="31"/>
       <c r="K31" s="44"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="96" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="109"/>
       <c r="D32" s="28"/>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -2071,7 +2063,7 @@
       <c r="J32" s="31"/>
       <c r="K32" s="44"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="23"/>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -2084,12 +2076,12 @@
       <c r="J33" s="31"/>
       <c r="K33" s="44"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="95"/>
-      <c r="C34" s="95"/>
+    <row r="34" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A34" s="106" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="107"/>
+      <c r="C34" s="107"/>
       <c r="D34" s="28"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
@@ -2099,12 +2091,12 @@
       <c r="J34" s="31"/>
       <c r="K34" s="44"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="92" t="s">
+    <row r="35" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A35" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="93"/>
+      <c r="B35" s="105"/>
+      <c r="C35" s="105"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
@@ -2114,7 +2106,7 @@
       <c r="J35" s="31"/>
       <c r="K35" s="44"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="23"/>
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
@@ -2127,7 +2119,7 @@
       <c r="J36" s="31"/>
       <c r="K36" s="44"/>
     </row>
-    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="46"/>
       <c r="B37" s="41"/>
       <c r="C37" s="41"/>
@@ -2140,7 +2132,7 @@
       <c r="J37" s="31"/>
       <c r="K37" s="44"/>
     </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -2153,22 +2145,22 @@
       <c r="J38" s="31"/>
       <c r="K38" s="44"/>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="77"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="78"/>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="90"/>
+      <c r="C39" s="90"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="91"/>
       <c r="I39" s="31"/>
       <c r="J39" s="31"/>
       <c r="K39" s="44"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="32"/>
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
@@ -2181,15 +2173,15 @@
       <c r="J40" s="31"/>
       <c r="K40" s="44"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="111"/>
+      <c r="C41" s="111"/>
       <c r="D41" s="28"/>
       <c r="E41" s="35" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F41" s="28"/>
       <c r="G41" s="24"/>
@@ -2198,12 +2190,12 @@
       <c r="J41" s="31"/>
       <c r="K41" s="44"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="101"/>
-      <c r="C42" s="102"/>
+    <row r="42" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A42" s="112" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="113"/>
+      <c r="C42" s="114"/>
       <c r="D42" s="28"/>
       <c r="E42" s="36"/>
       <c r="F42" s="28"/>
@@ -2213,9 +2205,9 @@
       <c r="J42" s="31"/>
       <c r="K42" s="44"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="47" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B43" s="34"/>
       <c r="C43" s="34"/>
@@ -2228,9 +2220,9 @@
       <c r="J43" s="31"/>
       <c r="K43" s="44"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B44" s="34"/>
       <c r="C44" s="34"/>
@@ -2243,7 +2235,7 @@
       <c r="J44" s="31"/>
       <c r="K44" s="44"/>
     </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="48"/>
       <c r="B45" s="41"/>
       <c r="C45" s="41"/>
@@ -2256,7 +2248,7 @@
       <c r="J45" s="31"/>
       <c r="K45" s="44"/>
     </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -2270,26 +2262,26 @@
       <c r="K46" s="44"/>
     </row>
     <row r="47" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="78"/>
+      <c r="A47" s="89" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="90"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="91"/>
       <c r="I47" s="31"/>
       <c r="J47" s="31"/>
       <c r="K47" s="44"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="32"/>
       <c r="B48" s="31"/>
       <c r="C48" s="31"/>
       <c r="D48" s="31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E48" s="31"/>
       <c r="F48" s="31"/>
@@ -2299,11 +2291,11 @@
       <c r="J48" s="31"/>
       <c r="K48" s="44"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="123" t="s">
-        <v>123</v>
-      </c>
-      <c r="B49" s="124"/>
+    <row r="49" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A49" s="85" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="86"/>
       <c r="C49" s="31"/>
       <c r="D49" s="31"/>
       <c r="E49" s="31"/>
@@ -2314,12 +2306,12 @@
       <c r="J49" s="31"/>
       <c r="K49" s="44"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="49" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B50" s="43" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
@@ -2331,7 +2323,7 @@
       <c r="J50" s="31"/>
       <c r="K50" s="44"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="32"/>
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
@@ -2344,7 +2336,7 @@
       <c r="J51" s="31"/>
       <c r="K51" s="44"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="32"/>
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
@@ -2357,11 +2349,11 @@
       <c r="J52" s="31"/>
       <c r="K52" s="44"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="125" t="s">
-        <v>120</v>
-      </c>
-      <c r="B53" s="126"/>
+    <row r="53" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A53" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="88"/>
       <c r="C53" s="31"/>
       <c r="D53" s="31"/>
       <c r="E53" s="31"/>
@@ -2372,12 +2364,12 @@
       <c r="J53" s="31"/>
       <c r="K53" s="44"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="50" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="31"/>
@@ -2389,7 +2381,7 @@
       <c r="J54" s="31"/>
       <c r="K54" s="44"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="32"/>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -2402,11 +2394,11 @@
       <c r="J55" s="31"/>
       <c r="K55" s="44"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="127" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="128"/>
+    <row r="56" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A56" s="92" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="93"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
@@ -2417,11 +2409,11 @@
       <c r="J56" s="31"/>
       <c r="K56" s="44"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="129" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" s="130"/>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="95"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
@@ -2432,7 +2424,7 @@
       <c r="J57" s="31"/>
       <c r="K57" s="44"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="32"/>
       <c r="B58" s="31"/>
       <c r="C58" s="31"/>
@@ -2445,7 +2437,7 @@
       <c r="J58" s="31"/>
       <c r="K58" s="44"/>
     </row>
-    <row r="59" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="46"/>
       <c r="B59" s="41"/>
       <c r="C59" s="41"/>
@@ -2458,7 +2450,7 @@
       <c r="J59" s="31"/>
       <c r="K59" s="44"/>
     </row>
-    <row r="60" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="23"/>
       <c r="B60" s="24"/>
       <c r="C60" s="24"/>
@@ -2471,22 +2463,22 @@
       <c r="J60" s="31"/>
       <c r="K60" s="44"/>
     </row>
-    <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="76" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="77"/>
-      <c r="C61" s="77"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="77"/>
-      <c r="F61" s="77"/>
-      <c r="G61" s="77"/>
-      <c r="H61" s="78"/>
+    <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="89" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="90"/>
+      <c r="C61" s="90"/>
+      <c r="D61" s="90"/>
+      <c r="E61" s="90"/>
+      <c r="F61" s="90"/>
+      <c r="G61" s="90"/>
+      <c r="H61" s="91"/>
       <c r="I61" s="31"/>
       <c r="J61" s="31"/>
       <c r="K61" s="44"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="23"/>
       <c r="B62" s="24"/>
       <c r="C62" s="24"/>
@@ -2499,38 +2491,36 @@
       <c r="J62" s="31"/>
       <c r="K62" s="44"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="105" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="106"/>
-      <c r="C63" s="106"/>
-      <c r="D63" s="106"/>
-      <c r="E63" s="106"/>
+    <row r="63" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A63" s="117" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" s="118"/>
+      <c r="C63" s="118"/>
+      <c r="D63" s="118"/>
+      <c r="E63" s="118"/>
       <c r="F63" s="31"/>
-      <c r="G63" s="24" t="s">
-        <v>43</v>
-      </c>
+      <c r="G63" s="24"/>
       <c r="H63" s="40"/>
       <c r="I63" s="31"/>
       <c r="J63" s="31"/>
       <c r="K63" s="44"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F64" s="24"/>
       <c r="G64" s="24"/>
@@ -2539,21 +2529,21 @@
       <c r="J64" s="31"/>
       <c r="K64" s="44"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F65" s="24"/>
       <c r="G65" s="24"/>
@@ -2562,7 +2552,7 @@
       <c r="J65" s="31"/>
       <c r="K65" s="44"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="23"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
@@ -2575,14 +2565,14 @@
       <c r="J66" s="31"/>
       <c r="K66" s="44"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" s="107" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="108"/>
-      <c r="C67" s="108"/>
-      <c r="D67" s="108"/>
-      <c r="E67" s="109"/>
+    <row r="67" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A67" s="119" t="s">
+        <v>152</v>
+      </c>
+      <c r="B67" s="120"/>
+      <c r="C67" s="120"/>
+      <c r="D67" s="120"/>
+      <c r="E67" s="121"/>
       <c r="F67" s="24"/>
       <c r="G67" s="31"/>
       <c r="H67" s="40"/>
@@ -2590,21 +2580,21 @@
       <c r="J67" s="31"/>
       <c r="K67" s="44"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F68" s="24"/>
       <c r="G68" s="24"/>
@@ -2613,7 +2603,7 @@
       <c r="J68" s="31"/>
       <c r="K68" s="44"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="58" t="str">
         <f>A65</f>
         <v>- dane z sensorów</v>
@@ -2641,7 +2631,7 @@
       <c r="J69" s="31"/>
       <c r="K69" s="44"/>
     </row>
-    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="46"/>
       <c r="B70" s="41"/>
       <c r="C70" s="41"/>
@@ -2654,7 +2644,7 @@
       <c r="J70" s="31"/>
       <c r="K70" s="44"/>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="23"/>
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
@@ -2667,22 +2657,22 @@
       <c r="J71" s="31"/>
       <c r="K71" s="44"/>
     </row>
-    <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="B72" s="77"/>
-      <c r="C72" s="77"/>
-      <c r="D72" s="77"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="77"/>
-      <c r="G72" s="77"/>
-      <c r="H72" s="78"/>
+    <row r="72" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="90"/>
+      <c r="C72" s="90"/>
+      <c r="D72" s="90"/>
+      <c r="E72" s="90"/>
+      <c r="F72" s="90"/>
+      <c r="G72" s="90"/>
+      <c r="H72" s="91"/>
       <c r="I72" s="31"/>
       <c r="J72" s="31"/>
       <c r="K72" s="44"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="23"/>
       <c r="B73" s="24"/>
       <c r="C73" s="24"/>
@@ -2695,12 +2685,12 @@
       <c r="J73" s="31"/>
       <c r="K73" s="44"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" s="79" t="s">
-        <v>62</v>
-      </c>
-      <c r="B74" s="80"/>
-      <c r="C74" s="80"/>
+    <row r="74" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A74" s="126" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="127"/>
+      <c r="C74" s="127"/>
       <c r="D74" s="24"/>
       <c r="E74" s="24"/>
       <c r="F74" s="24"/>
@@ -2710,15 +2700,15 @@
       <c r="J74" s="31"/>
       <c r="K74" s="44"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B75" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="C75" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D75" s="24"/>
       <c r="E75" s="24"/>
@@ -2729,18 +2719,18 @@
       <c r="J75" s="31"/>
       <c r="K75" s="44"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E76" s="24"/>
       <c r="F76" s="24"/>
@@ -2750,7 +2740,7 @@
       <c r="J76" s="31"/>
       <c r="K76" s="44"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="23"/>
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
@@ -2763,14 +2753,14 @@
       <c r="J77" s="31"/>
       <c r="K77" s="44"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="122" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" s="122"/>
-      <c r="C78" s="122"/>
-      <c r="D78" s="122"/>
-      <c r="E78" s="122"/>
+    <row r="78" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A78" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" s="84"/>
+      <c r="C78" s="84"/>
+      <c r="D78" s="84"/>
+      <c r="E78" s="84"/>
       <c r="F78" s="24"/>
       <c r="G78" s="24"/>
       <c r="H78" s="40"/>
@@ -2778,9 +2768,9 @@
       <c r="J78" s="31"/>
       <c r="K78" s="44"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>13</v>
@@ -2789,10 +2779,10 @@
         <v>14</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F79" s="24"/>
       <c r="G79" s="24"/>
@@ -2801,15 +2791,15 @@
       <c r="J79" s="31"/>
       <c r="K79" s="44"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="26" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B80" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D80" s="14" t="s">
         <v>17</v>
@@ -2822,7 +2812,7 @@
       <c r="J80" s="31"/>
       <c r="K80" s="44"/>
     </row>
-    <row r="81" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="46"/>
       <c r="B81" s="41"/>
       <c r="C81" s="41"/>
@@ -2835,7 +2825,7 @@
       <c r="J81" s="31"/>
       <c r="K81" s="44"/>
     </row>
-    <row r="82" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="32"/>
       <c r="B82" s="31"/>
       <c r="C82" s="31"/>
@@ -2848,22 +2838,22 @@
       <c r="J82" s="31"/>
       <c r="K82" s="44"/>
     </row>
-    <row r="83" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="76" t="s">
-        <v>116</v>
-      </c>
-      <c r="B83" s="77"/>
-      <c r="C83" s="77"/>
-      <c r="D83" s="77"/>
-      <c r="E83" s="77"/>
-      <c r="F83" s="77"/>
-      <c r="G83" s="77"/>
-      <c r="H83" s="78"/>
+    <row r="83" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" s="90"/>
+      <c r="C83" s="90"/>
+      <c r="D83" s="90"/>
+      <c r="E83" s="90"/>
+      <c r="F83" s="90"/>
+      <c r="G83" s="90"/>
+      <c r="H83" s="91"/>
       <c r="I83" s="31"/>
       <c r="J83" s="31"/>
       <c r="K83" s="44"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="23"/>
       <c r="B84" s="24"/>
       <c r="C84" s="24"/>
@@ -2876,11 +2866,11 @@
       <c r="J84" s="31"/>
       <c r="K84" s="44"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="B85" s="104"/>
+    <row r="85" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A85" s="115" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="116"/>
       <c r="C85" s="24"/>
       <c r="D85" s="24"/>
       <c r="E85" s="24"/>
@@ -2891,12 +2881,12 @@
       <c r="J85" s="31"/>
       <c r="K85" s="44"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="45" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C86" s="24"/>
       <c r="D86" s="24"/>
@@ -2908,7 +2898,7 @@
       <c r="J86" s="31"/>
       <c r="K86" s="44"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="23"/>
       <c r="B87" s="24"/>
       <c r="C87" s="24"/>
@@ -2921,7 +2911,7 @@
       <c r="J87" s="31"/>
       <c r="K87" s="44"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="46"/>
       <c r="B88" s="41"/>
       <c r="C88" s="41"/>
@@ -2934,7 +2924,7 @@
       <c r="J88" s="31"/>
       <c r="K88" s="44"/>
     </row>
-    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="23"/>
       <c r="B89" s="24"/>
       <c r="C89" s="24"/>
@@ -2947,22 +2937,22 @@
       <c r="J89" s="31"/>
       <c r="K89" s="44"/>
     </row>
-    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="76" t="s">
-        <v>117</v>
-      </c>
-      <c r="B90" s="77"/>
-      <c r="C90" s="77"/>
-      <c r="D90" s="77"/>
-      <c r="E90" s="77"/>
-      <c r="F90" s="77"/>
-      <c r="G90" s="77"/>
-      <c r="H90" s="78"/>
+    <row r="90" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="89" t="s">
+        <v>112</v>
+      </c>
+      <c r="B90" s="90"/>
+      <c r="C90" s="90"/>
+      <c r="D90" s="90"/>
+      <c r="E90" s="90"/>
+      <c r="F90" s="90"/>
+      <c r="G90" s="90"/>
+      <c r="H90" s="91"/>
       <c r="I90" s="31"/>
       <c r="J90" s="31"/>
       <c r="K90" s="44"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="23"/>
       <c r="B91" s="24"/>
       <c r="C91" s="24"/>
@@ -2975,15 +2965,15 @@
       <c r="J91" s="31"/>
       <c r="K91" s="44"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="B92" s="120"/>
-      <c r="C92" s="120"/>
-      <c r="D92" s="121"/>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="81" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="82"/>
+      <c r="C92" s="82"/>
+      <c r="D92" s="83"/>
       <c r="E92" s="28" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F92" s="28"/>
       <c r="G92" s="28"/>
@@ -2992,18 +2982,18 @@
       <c r="J92" s="31"/>
       <c r="K92" s="44"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="51" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B93" s="62" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E93" s="28"/>
       <c r="F93" s="28"/>
@@ -3013,18 +3003,18 @@
       <c r="J93" s="31"/>
       <c r="K93" s="44"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B94" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C94" s="24" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D94" s="24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E94" s="28"/>
       <c r="F94" s="28"/>
@@ -3034,7 +3024,7 @@
       <c r="J94" s="31"/>
       <c r="K94" s="44"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="23"/>
       <c r="B95" s="24"/>
       <c r="C95" s="24"/>
@@ -3047,11 +3037,11 @@
       <c r="J95" s="31"/>
       <c r="K95" s="44"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A96" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" s="87"/>
+    <row r="96" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A96" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" s="99"/>
       <c r="C96" s="24"/>
       <c r="D96" s="28"/>
       <c r="E96" s="28"/>
@@ -3062,12 +3052,12 @@
       <c r="J96" s="31"/>
       <c r="K96" s="44"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="52" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C97" s="24"/>
       <c r="D97" s="28"/>
@@ -3079,9 +3069,9 @@
       <c r="J97" s="31"/>
       <c r="K97" s="44"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B98" s="31"/>
       <c r="C98" s="31"/>
@@ -3094,7 +3084,7 @@
       <c r="J98" s="31"/>
       <c r="K98" s="44"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="32"/>
       <c r="B99" s="31"/>
       <c r="C99" s="31"/>
@@ -3107,11 +3097,11 @@
       <c r="J99" s="31"/>
       <c r="K99" s="44"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A100" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B100" s="89"/>
+    <row r="100" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A100" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="B100" s="101"/>
       <c r="C100" s="31"/>
       <c r="D100" s="36"/>
       <c r="E100" s="36"/>
@@ -3122,12 +3112,12 @@
       <c r="J100" s="31"/>
       <c r="K100" s="44"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="53" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="36"/>
@@ -3139,9 +3129,9 @@
       <c r="J101" s="31"/>
       <c r="K101" s="44"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="32" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B102" s="31" t="s">
         <v>9</v>
@@ -3156,7 +3146,7 @@
       <c r="J102" s="31"/>
       <c r="K102" s="44"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="46"/>
       <c r="B103" s="41"/>
       <c r="C103" s="41"/>
@@ -3169,7 +3159,7 @@
       <c r="J103" s="31"/>
       <c r="K103" s="44"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="32"/>
       <c r="B104" s="31"/>
       <c r="C104" s="31"/>
@@ -3182,22 +3172,22 @@
       <c r="J104" s="31"/>
       <c r="K104" s="44"/>
     </row>
-    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="77"/>
-      <c r="C105" s="77"/>
-      <c r="D105" s="77"/>
-      <c r="E105" s="77"/>
-      <c r="F105" s="77"/>
-      <c r="G105" s="77"/>
-      <c r="H105" s="78"/>
+    <row r="105" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="90"/>
+      <c r="C105" s="90"/>
+      <c r="D105" s="90"/>
+      <c r="E105" s="90"/>
+      <c r="F105" s="90"/>
+      <c r="G105" s="90"/>
+      <c r="H105" s="91"/>
       <c r="I105" s="31"/>
       <c r="J105" s="31"/>
       <c r="K105" s="44"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="23"/>
       <c r="B106" s="24"/>
       <c r="C106" s="24"/>
@@ -3210,15 +3200,15 @@
       <c r="J106" s="31"/>
       <c r="K106" s="44"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A107" s="116" t="s">
-        <v>111</v>
-      </c>
-      <c r="B107" s="117"/>
-      <c r="C107" s="118"/>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" s="79"/>
+      <c r="C107" s="80"/>
       <c r="D107" s="28"/>
       <c r="E107" s="28" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F107" s="31"/>
       <c r="G107" s="31"/>
@@ -3227,15 +3217,15 @@
       <c r="J107" s="31"/>
       <c r="K107" s="44"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="54" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -3246,15 +3236,15 @@
       <c r="J108" s="31"/>
       <c r="K108" s="44"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B109" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D109" s="28"/>
       <c r="E109" s="28"/>
@@ -3265,7 +3255,7 @@
       <c r="J109" s="31"/>
       <c r="K109" s="44"/>
     </row>
-    <row r="110" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="46"/>
       <c r="B110" s="41"/>
       <c r="C110" s="41"/>
@@ -3278,7 +3268,7 @@
       <c r="J110" s="31"/>
       <c r="K110" s="44"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="32"/>
       <c r="B111" s="31"/>
       <c r="C111" s="31"/>
@@ -3291,7 +3281,7 @@
       <c r="J111" s="31"/>
       <c r="K111" s="44"/>
     </row>
-    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="23"/>
       <c r="B112" s="24"/>
       <c r="C112" s="24"/>
@@ -3304,22 +3294,22 @@
       <c r="J112" s="31"/>
       <c r="K112" s="44"/>
     </row>
-    <row r="113" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="B113" s="77"/>
-      <c r="C113" s="77"/>
-      <c r="D113" s="77"/>
-      <c r="E113" s="77"/>
-      <c r="F113" s="77"/>
-      <c r="G113" s="77"/>
-      <c r="H113" s="78"/>
+    <row r="113" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="89" t="s">
+        <v>110</v>
+      </c>
+      <c r="B113" s="90"/>
+      <c r="C113" s="90"/>
+      <c r="D113" s="90"/>
+      <c r="E113" s="90"/>
+      <c r="F113" s="90"/>
+      <c r="G113" s="90"/>
+      <c r="H113" s="91"/>
       <c r="I113" s="31"/>
       <c r="J113" s="31"/>
       <c r="K113" s="44"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="23"/>
       <c r="B114" s="24"/>
       <c r="C114" s="24"/>
@@ -3332,14 +3322,14 @@
       <c r="J114" s="31"/>
       <c r="K114" s="44"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A115" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="B115" s="75"/>
-      <c r="C115" s="75"/>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="124" t="s">
+        <v>61</v>
+      </c>
+      <c r="B115" s="125"/>
+      <c r="C115" s="125"/>
       <c r="D115" s="35" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F115" s="24"/>
       <c r="G115" s="24"/>
@@ -3348,15 +3338,15 @@
       <c r="J115" s="31"/>
       <c r="K115" s="44"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B116" s="22" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C116" s="61" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D116" s="24"/>
       <c r="E116" s="24"/>
@@ -3367,12 +3357,12 @@
       <c r="J116" s="31"/>
       <c r="K116" s="44"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B117" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C117" s="24"/>
       <c r="D117" s="24"/>
@@ -3384,7 +3374,7 @@
       <c r="J117" s="31"/>
       <c r="K117" s="44"/>
     </row>
-    <row r="118" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="46"/>
       <c r="B118" s="41"/>
       <c r="C118" s="41"/>
@@ -3397,7 +3387,7 @@
       <c r="J118" s="31"/>
       <c r="K118" s="44"/>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="32"/>
       <c r="B119" s="31"/>
       <c r="C119" s="31"/>
@@ -3410,25 +3400,25 @@
       <c r="J119" s="31"/>
       <c r="K119" s="44"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A120" s="81" t="s">
-        <v>146</v>
-      </c>
-      <c r="B120" s="82"/>
-      <c r="C120" s="82"/>
-      <c r="D120" s="82"/>
-      <c r="E120" s="82"/>
-      <c r="F120" s="82"/>
-      <c r="G120" s="82"/>
-      <c r="H120" s="83"/>
+    <row r="120" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A120" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="B120" s="129"/>
+      <c r="C120" s="129"/>
+      <c r="D120" s="129"/>
+      <c r="E120" s="129"/>
+      <c r="F120" s="129"/>
+      <c r="G120" s="129"/>
+      <c r="H120" s="130"/>
       <c r="I120" s="31"/>
       <c r="J120" s="31"/>
       <c r="K120" s="44"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="64"/>
       <c r="B121" s="70" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C121" s="71"/>
       <c r="D121" s="31"/>
@@ -3440,13 +3430,13 @@
       <c r="J121" s="31"/>
       <c r="K121" s="44"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="64"/>
       <c r="B122" s="66" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C122" s="63" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D122" s="31"/>
       <c r="E122" s="31"/>
@@ -3457,13 +3447,13 @@
       <c r="J122" s="31"/>
       <c r="K122" s="44"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A123" s="72" t="s">
-        <v>149</v>
-      </c>
-      <c r="B123" s="73"/>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="122" t="s">
+        <v>144</v>
+      </c>
+      <c r="B123" s="123"/>
       <c r="C123" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D123" s="31"/>
       <c r="E123" s="31"/>
@@ -3474,12 +3464,12 @@
       <c r="J123" s="31"/>
       <c r="K123" s="44"/>
     </row>
-    <row r="124" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="67"/>
       <c r="B124" s="68"/>
       <c r="C124" s="68"/>
       <c r="D124" s="68" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E124" s="68"/>
       <c r="F124" s="68"/>
@@ -3489,7 +3479,7 @@
       <c r="J124" s="31"/>
       <c r="K124" s="44"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="31"/>
       <c r="B125" s="31"/>
       <c r="C125" s="31"/>
@@ -3502,7 +3492,7 @@
       <c r="J125" s="31"/>
       <c r="K125" s="44"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="31"/>
       <c r="B126" s="31"/>
       <c r="C126" s="31"/>
@@ -3515,7 +3505,7 @@
       <c r="J126" s="31"/>
       <c r="K126" s="44"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127" s="31"/>
       <c r="B127" s="31"/>
       <c r="C127" s="31"/>
@@ -3528,7 +3518,7 @@
       <c r="J127" s="31"/>
       <c r="K127" s="44"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128" s="32"/>
       <c r="B128" s="31"/>
       <c r="C128" s="31"/>
@@ -3541,7 +3531,7 @@
       <c r="J128" s="31"/>
       <c r="K128" s="44"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="32"/>
       <c r="B129" s="31"/>
       <c r="C129" s="31"/>
@@ -3554,7 +3544,7 @@
       <c r="J129" s="31"/>
       <c r="K129" s="44"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130" s="32"/>
       <c r="B130" s="31"/>
       <c r="C130" s="31"/>
@@ -3567,7 +3557,7 @@
       <c r="J130" s="31"/>
       <c r="K130" s="44"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131" s="32"/>
       <c r="B131" s="31"/>
       <c r="C131" s="31"/>
@@ -3580,7 +3570,7 @@
       <c r="J131" s="31"/>
       <c r="K131" s="44"/>
     </row>
-    <row r="132" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="33"/>
       <c r="B132" s="55"/>
       <c r="C132" s="55"/>
@@ -3595,6 +3585,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A115:C115"/>
+    <mergeCell ref="A113:H113"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A120:H120"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A67:E67"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="E19:E22"/>
@@ -3611,25 +3620,6 @@
     <mergeCell ref="A83:H83"/>
     <mergeCell ref="A90:H90"/>
     <mergeCell ref="A105:H105"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A115:C115"/>
-    <mergeCell ref="A113:H113"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A120:H120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3644,12 +3634,12 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="141" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3659,47 +3649,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3709,47 +3699,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -3768,36 +3758,36 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>